<commit_message>
add pdf to kml zip package
</commit_message>
<xml_diff>
--- a/misc data/Legends2.xlsx
+++ b/misc data/Legends2.xlsx
@@ -249,6 +249,129 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>427380</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>129457</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>442633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="C:\Users\lfortini\Dropbox\USGS\Science\0-ongoing\VAs\VA Products\WSC\HCA Logos\HCA Logos\logo_USGS.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="15724" b="9563"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1850527" y="1882588"/>
+          <a:ext cx="923518" cy="431427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5603</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>459011</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>417730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="C:\Users\lfortini\Downloads\PICCC ppt logo horizontal.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="616324" y="1880549"/>
+          <a:ext cx="1265834" cy="408563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +864,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -856,6 +979,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>